<commit_message>
Some badass shit here with my watchlist creatot GUI...
</commit_message>
<xml_diff>
--- a/User_Data/NLQ_Data/NLQ_Data.xlsx
+++ b/User_Data/NLQ_Data/NLQ_Data.xlsx
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B181"/>
+  <dimension ref="A1:B187"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1899,6 +1899,54 @@
         <v>6137.827</v>
       </c>
     </row>
+    <row r="182">
+      <c r="A182" s="3" t="n">
+        <v>45469</v>
+      </c>
+      <c r="B182" t="n">
+        <v>5975.589999999999</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="3" t="n">
+        <v>45476</v>
+      </c>
+      <c r="B183" t="n">
+        <v>6034.249000000001</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="3" t="n">
+        <v>45483</v>
+      </c>
+      <c r="B184" t="n">
+        <v>6065.53</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="3" t="n">
+        <v>45490</v>
+      </c>
+      <c r="B185" t="n">
+        <v>6057.253000000001</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="3" t="n">
+        <v>45497</v>
+      </c>
+      <c r="B186" t="n">
+        <v>6032.018999999999</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="3" t="n">
+        <v>45504</v>
+      </c>
+      <c r="B187" t="n">
+        <v>5978.705</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1910,7 +1958,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1273"/>
+  <dimension ref="A1:B1312"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12098,7 +12146,319 @@
         <v>45468</v>
       </c>
       <c r="B1273" t="n">
-        <v>6093.216</v>
+        <v>6062.822</v>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" s="3" t="n">
+        <v>45469</v>
+      </c>
+      <c r="B1274" t="n">
+        <v>5975.589999999999</v>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" s="3" t="n">
+        <v>45470</v>
+      </c>
+      <c r="B1275" t="n">
+        <v>5934.053999999999</v>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" s="3" t="n">
+        <v>45471</v>
+      </c>
+      <c r="B1276" t="n">
+        <v>5801.175999999999</v>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" s="3" t="n">
+        <v>45472</v>
+      </c>
+      <c r="B1277" t="n">
+        <v>5801.175999999999</v>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" s="3" t="n">
+        <v>45473</v>
+      </c>
+      <c r="B1278" t="n">
+        <v>5801.175999999999</v>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" s="3" t="n">
+        <v>45474</v>
+      </c>
+      <c r="B1279" t="n">
+        <v>6013.962999999999</v>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" s="3" t="n">
+        <v>45475</v>
+      </c>
+      <c r="B1280" t="n">
+        <v>6022.376999999999</v>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" s="3" t="n">
+        <v>45476</v>
+      </c>
+      <c r="B1281" t="n">
+        <v>6034.249000000001</v>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" s="3" t="n">
+        <v>45477</v>
+      </c>
+      <c r="B1282" t="n">
+        <v>6034.249000000001</v>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" s="3" t="n">
+        <v>45478</v>
+      </c>
+      <c r="B1283" t="n">
+        <v>6069.515000000001</v>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" s="3" t="n">
+        <v>45479</v>
+      </c>
+      <c r="B1284" t="n">
+        <v>6069.515000000001</v>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" s="3" t="n">
+        <v>45480</v>
+      </c>
+      <c r="B1285" t="n">
+        <v>6069.515000000001</v>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" s="3" t="n">
+        <v>45481</v>
+      </c>
+      <c r="B1286" t="n">
+        <v>6044.890000000001</v>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" s="3" t="n">
+        <v>45482</v>
+      </c>
+      <c r="B1287" t="n">
+        <v>6036.995000000001</v>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" s="3" t="n">
+        <v>45483</v>
+      </c>
+      <c r="B1288" t="n">
+        <v>6065.53</v>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" s="3" t="n">
+        <v>45484</v>
+      </c>
+      <c r="B1289" t="n">
+        <v>6083.969</v>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" s="3" t="n">
+        <v>45485</v>
+      </c>
+      <c r="B1290" t="n">
+        <v>6081.087</v>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" s="3" t="n">
+        <v>45486</v>
+      </c>
+      <c r="B1291" t="n">
+        <v>6081.087</v>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" s="3" t="n">
+        <v>45487</v>
+      </c>
+      <c r="B1292" t="n">
+        <v>6081.087</v>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" s="3" t="n">
+        <v>45488</v>
+      </c>
+      <c r="B1293" t="n">
+        <v>6074.397</v>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" s="3" t="n">
+        <v>45489</v>
+      </c>
+      <c r="B1294" t="n">
+        <v>6078.083</v>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" s="3" t="n">
+        <v>45490</v>
+      </c>
+      <c r="B1295" t="n">
+        <v>6057.253000000001</v>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" s="3" t="n">
+        <v>45491</v>
+      </c>
+      <c r="B1296" t="n">
+        <v>6065.002</v>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" s="3" t="n">
+        <v>45492</v>
+      </c>
+      <c r="B1297" t="n">
+        <v>6076.853</v>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" s="3" t="n">
+        <v>45493</v>
+      </c>
+      <c r="B1298" t="n">
+        <v>6076.853</v>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" s="3" t="n">
+        <v>45494</v>
+      </c>
+      <c r="B1299" t="n">
+        <v>6076.853</v>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" s="3" t="n">
+        <v>45495</v>
+      </c>
+      <c r="B1300" t="n">
+        <v>6060.753000000001</v>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" s="3" t="n">
+        <v>45496</v>
+      </c>
+      <c r="B1301" t="n">
+        <v>6066.817000000001</v>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" s="3" t="n">
+        <v>45497</v>
+      </c>
+      <c r="B1302" t="n">
+        <v>6032.018999999999</v>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" s="3" t="n">
+        <v>45498</v>
+      </c>
+      <c r="B1303" t="n">
+        <v>6053.706999999999</v>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" s="3" t="n">
+        <v>45499</v>
+      </c>
+      <c r="B1304" t="n">
+        <v>6049.883</v>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" s="3" t="n">
+        <v>45500</v>
+      </c>
+      <c r="B1305" t="n">
+        <v>6049.883</v>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" s="3" t="n">
+        <v>45501</v>
+      </c>
+      <c r="B1306" t="n">
+        <v>6049.883</v>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" s="3" t="n">
+        <v>45502</v>
+      </c>
+      <c r="B1307" t="n">
+        <v>6045.858999999999</v>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" s="3" t="n">
+        <v>45503</v>
+      </c>
+      <c r="B1308" t="n">
+        <v>6064.085999999999</v>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" s="3" t="n">
+        <v>45504</v>
+      </c>
+      <c r="B1309" t="n">
+        <v>5978.705</v>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" s="3" t="n">
+        <v>45505</v>
+      </c>
+      <c r="B1310" t="n">
+        <v>6043.02</v>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" s="3" t="n">
+        <v>45506</v>
+      </c>
+      <c r="B1311" t="n">
+        <v>6053.432</v>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" s="3" t="n">
+        <v>45507</v>
+      </c>
+      <c r="B1312" t="n">
+        <v>6053.432</v>
       </c>
     </row>
   </sheetData>
@@ -12112,7 +12472,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1273"/>
+  <dimension ref="A1:B1312"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22108,7 +22468,7 @@
         <v>45444</v>
       </c>
       <c r="B1249" t="n">
-        <v>6245.260485049961</v>
+        <v>6236.26155736826</v>
       </c>
     </row>
     <row r="1250">
@@ -22116,7 +22476,7 @@
         <v>45445</v>
       </c>
       <c r="B1250" t="n">
-        <v>6245.260485049961</v>
+        <v>6236.26155736826</v>
       </c>
     </row>
     <row r="1251">
@@ -22124,7 +22484,7 @@
         <v>45446</v>
       </c>
       <c r="B1251" t="n">
-        <v>6304.56448504996</v>
+        <v>6295.565557368259</v>
       </c>
     </row>
     <row r="1252">
@@ -22132,7 +22492,7 @@
         <v>45447</v>
       </c>
       <c r="B1252" t="n">
-        <v>6325.515485049961</v>
+        <v>6316.51655736826</v>
       </c>
     </row>
     <row r="1253">
@@ -22140,7 +22500,7 @@
         <v>45448</v>
       </c>
       <c r="B1253" t="n">
-        <v>6299.755770764245</v>
+        <v>6290.756843082544</v>
       </c>
     </row>
     <row r="1254">
@@ -22148,7 +22508,7 @@
         <v>45449</v>
       </c>
       <c r="B1254" t="n">
-        <v>6316.039770764246</v>
+        <v>6307.040843082545</v>
       </c>
     </row>
     <row r="1255">
@@ -22156,7 +22516,7 @@
         <v>45450</v>
       </c>
       <c r="B1255" t="n">
-        <v>6303.940770764247</v>
+        <v>6294.941843082545</v>
       </c>
     </row>
     <row r="1256">
@@ -22164,7 +22524,7 @@
         <v>45451</v>
       </c>
       <c r="B1256" t="n">
-        <v>6303.940770764247</v>
+        <v>6294.941843082545</v>
       </c>
     </row>
     <row r="1257">
@@ -22172,7 +22532,7 @@
         <v>45452</v>
       </c>
       <c r="B1257" t="n">
-        <v>6303.940770764247</v>
+        <v>6294.941843082545</v>
       </c>
     </row>
     <row r="1258">
@@ -22180,7 +22540,7 @@
         <v>45453</v>
       </c>
       <c r="B1258" t="n">
-        <v>6268.120770764246</v>
+        <v>6259.121843082545</v>
       </c>
     </row>
     <row r="1259">
@@ -22188,7 +22548,7 @@
         <v>45454</v>
       </c>
       <c r="B1259" t="n">
-        <v>6297.243770764247</v>
+        <v>6288.244843082545</v>
       </c>
     </row>
     <row r="1260">
@@ -22196,7 +22556,7 @@
         <v>45455</v>
       </c>
       <c r="B1260" t="n">
-        <v>6280.302485049961</v>
+        <v>6271.30355736826</v>
       </c>
     </row>
     <row r="1261">
@@ -22204,7 +22564,7 @@
         <v>45456</v>
       </c>
       <c r="B1261" t="n">
-        <v>6300.197485049961</v>
+        <v>6291.19855736826</v>
       </c>
     </row>
     <row r="1262">
@@ -22212,7 +22572,7 @@
         <v>45457</v>
       </c>
       <c r="B1262" t="n">
-        <v>6314.89848504996</v>
+        <v>6305.899557368259</v>
       </c>
     </row>
     <row r="1263">
@@ -22220,7 +22580,7 @@
         <v>45458</v>
       </c>
       <c r="B1263" t="n">
-        <v>6314.89848504996</v>
+        <v>6305.899557368259</v>
       </c>
     </row>
     <row r="1264">
@@ -22228,7 +22588,7 @@
         <v>45459</v>
       </c>
       <c r="B1264" t="n">
-        <v>6314.89848504996</v>
+        <v>6305.899557368259</v>
       </c>
     </row>
     <row r="1265">
@@ -22236,7 +22596,7 @@
         <v>45460</v>
       </c>
       <c r="B1265" t="n">
-        <v>6222.04748504996</v>
+        <v>6213.048557368259</v>
       </c>
     </row>
     <row r="1266">
@@ -22244,7 +22604,7 @@
         <v>45461</v>
       </c>
       <c r="B1266" t="n">
-        <v>6220.38848504996</v>
+        <v>6211.389557368258</v>
       </c>
     </row>
     <row r="1267">
@@ -22252,7 +22612,7 @@
         <v>45462</v>
       </c>
       <c r="B1267" t="n">
-        <v>6213.603913621389</v>
+        <v>6204.604985939687</v>
       </c>
     </row>
     <row r="1268">
@@ -22260,7 +22620,7 @@
         <v>45463</v>
       </c>
       <c r="B1268" t="n">
-        <v>6210.713913621389</v>
+        <v>6201.714985939688</v>
       </c>
     </row>
     <row r="1269">
@@ -22268,7 +22628,7 @@
         <v>45464</v>
       </c>
       <c r="B1269" t="n">
-        <v>6186.837913621389</v>
+        <v>6177.838985939688</v>
       </c>
     </row>
     <row r="1270">
@@ -22276,7 +22636,7 @@
         <v>45465</v>
       </c>
       <c r="B1270" t="n">
-        <v>6186.837913621389</v>
+        <v>6177.838985939688</v>
       </c>
     </row>
     <row r="1271">
@@ -22284,7 +22644,7 @@
         <v>45466</v>
       </c>
       <c r="B1271" t="n">
-        <v>6186.837913621389</v>
+        <v>6177.838985939688</v>
       </c>
     </row>
     <row r="1272">
@@ -22292,7 +22652,7 @@
         <v>45467</v>
       </c>
       <c r="B1272" t="n">
-        <v>6171.961913621389</v>
+        <v>6141.954985939688</v>
       </c>
     </row>
     <row r="1273">
@@ -22300,7 +22660,319 @@
         <v>45468</v>
       </c>
       <c r="B1273" t="n">
-        <v>6171.961913621389</v>
+        <v>6128.745985939688</v>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" s="3" t="n">
+        <v>45469</v>
+      </c>
+      <c r="B1274" t="n">
+        <v>6105.844700225402</v>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" s="3" t="n">
+        <v>45470</v>
+      </c>
+      <c r="B1275" t="n">
+        <v>6089.896700225401</v>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" s="3" t="n">
+        <v>45471</v>
+      </c>
+      <c r="B1276" t="n">
+        <v>5897.838700225402</v>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" s="3" t="n">
+        <v>45472</v>
+      </c>
+      <c r="B1277" t="n">
+        <v>5897.838700225402</v>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" s="3" t="n">
+        <v>45473</v>
+      </c>
+      <c r="B1278" t="n">
+        <v>5897.838700225402</v>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" s="3" t="n">
+        <v>45474</v>
+      </c>
+      <c r="B1279" t="n">
+        <v>6124.984700225401</v>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" s="3" t="n">
+        <v>45475</v>
+      </c>
+      <c r="B1280" t="n">
+        <v>6128.283700225402</v>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" s="3" t="n">
+        <v>45476</v>
+      </c>
+      <c r="B1281" t="n">
+        <v>6158.634128796831</v>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" s="3" t="n">
+        <v>45477</v>
+      </c>
+      <c r="B1282" t="n">
+        <v>6158.634128796831</v>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" s="3" t="n">
+        <v>45478</v>
+      </c>
+      <c r="B1283" t="n">
+        <v>6207.349128796832</v>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" s="3" t="n">
+        <v>45479</v>
+      </c>
+      <c r="B1284" t="n">
+        <v>6207.349128796832</v>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" s="3" t="n">
+        <v>45480</v>
+      </c>
+      <c r="B1285" t="n">
+        <v>6207.349128796832</v>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" s="3" t="n">
+        <v>45481</v>
+      </c>
+      <c r="B1286" t="n">
+        <v>6171.715128796832</v>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" s="3" t="n">
+        <v>45482</v>
+      </c>
+      <c r="B1287" t="n">
+        <v>6159.750128796831</v>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" s="3" t="n">
+        <v>45483</v>
+      </c>
+      <c r="B1288" t="n">
+        <v>6188.110700225402</v>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" s="3" t="n">
+        <v>45484</v>
+      </c>
+      <c r="B1289" t="n">
+        <v>6197.461700225402</v>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" s="3" t="n">
+        <v>45485</v>
+      </c>
+      <c r="B1290" t="n">
+        <v>6191.530700225401</v>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" s="3" t="n">
+        <v>45486</v>
+      </c>
+      <c r="B1291" t="n">
+        <v>6191.530700225401</v>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" s="3" t="n">
+        <v>45487</v>
+      </c>
+      <c r="B1292" t="n">
+        <v>6191.530700225401</v>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" s="3" t="n">
+        <v>45488</v>
+      </c>
+      <c r="B1293" t="n">
+        <v>6154.767700225401</v>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" s="3" t="n">
+        <v>45489</v>
+      </c>
+      <c r="B1294" t="n">
+        <v>6127.967700225401</v>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" s="3" t="n">
+        <v>45490</v>
+      </c>
+      <c r="B1295" t="n">
+        <v>6147.67155736826</v>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" s="3" t="n">
+        <v>45491</v>
+      </c>
+      <c r="B1296" t="n">
+        <v>6146.420557368259</v>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" s="3" t="n">
+        <v>45492</v>
+      </c>
+      <c r="B1297" t="n">
+        <v>6162.798557368259</v>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" s="3" t="n">
+        <v>45493</v>
+      </c>
+      <c r="B1298" t="n">
+        <v>6162.798557368259</v>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" s="3" t="n">
+        <v>45494</v>
+      </c>
+      <c r="B1299" t="n">
+        <v>6162.798557368259</v>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" s="3" t="n">
+        <v>45495</v>
+      </c>
+      <c r="B1300" t="n">
+        <v>6148.167557368259</v>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" s="3" t="n">
+        <v>45496</v>
+      </c>
+      <c r="B1301" t="n">
+        <v>6130.54755736826</v>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" s="3" t="n">
+        <v>45497</v>
+      </c>
+      <c r="B1302" t="n">
+        <v>6143.766700225402</v>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" s="3" t="n">
+        <v>45498</v>
+      </c>
+      <c r="B1303" t="n">
+        <v>6164.979700225402</v>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" s="3" t="n">
+        <v>45499</v>
+      </c>
+      <c r="B1304" t="n">
+        <v>6162.521700225402</v>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" s="3" t="n">
+        <v>45500</v>
+      </c>
+      <c r="B1305" t="n">
+        <v>6162.521700225402</v>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" s="3" t="n">
+        <v>45501</v>
+      </c>
+      <c r="B1306" t="n">
+        <v>6162.521700225402</v>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" s="3" t="n">
+        <v>45502</v>
+      </c>
+      <c r="B1307" t="n">
+        <v>6143.525700225402</v>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" s="3" t="n">
+        <v>45503</v>
+      </c>
+      <c r="B1308" t="n">
+        <v>6140.830700225401</v>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" s="3" t="n">
+        <v>45504</v>
+      </c>
+      <c r="B1309" t="n">
+        <v>6015.721557368259</v>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" s="3" t="n">
+        <v>45505</v>
+      </c>
+      <c r="B1310" t="n">
+        <v>6148.943557368259</v>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" s="3" t="n">
+        <v>45506</v>
+      </c>
+      <c r="B1311" t="n">
+        <v>6159.355557368259</v>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" s="3" t="n">
+        <v>45507</v>
+      </c>
+      <c r="B1312" t="n">
+        <v>6159.355557368259</v>
       </c>
     </row>
   </sheetData>
@@ -22314,7 +22986,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1273"/>
+  <dimension ref="A1:B1312"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -32505,6 +33177,318 @@
         <v>7252.542</v>
       </c>
     </row>
+    <row r="1274">
+      <c r="A1274" s="3" t="n">
+        <v>45469</v>
+      </c>
+      <c r="B1274" t="n">
+        <v>7231.163</v>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" s="3" t="n">
+        <v>45470</v>
+      </c>
+      <c r="B1275" t="n">
+        <v>7231.163</v>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" s="3" t="n">
+        <v>45471</v>
+      </c>
+      <c r="B1276" t="n">
+        <v>7231.163</v>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" s="3" t="n">
+        <v>45472</v>
+      </c>
+      <c r="B1277" t="n">
+        <v>7231.163</v>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" s="3" t="n">
+        <v>45473</v>
+      </c>
+      <c r="B1278" t="n">
+        <v>7231.163</v>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" s="3" t="n">
+        <v>45474</v>
+      </c>
+      <c r="B1279" t="n">
+        <v>7231.163</v>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" s="3" t="n">
+        <v>45475</v>
+      </c>
+      <c r="B1280" t="n">
+        <v>7231.163</v>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" s="3" t="n">
+        <v>45476</v>
+      </c>
+      <c r="B1281" t="n">
+        <v>7221.52</v>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" s="3" t="n">
+        <v>45477</v>
+      </c>
+      <c r="B1282" t="n">
+        <v>7221.52</v>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" s="3" t="n">
+        <v>45478</v>
+      </c>
+      <c r="B1283" t="n">
+        <v>7221.52</v>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" s="3" t="n">
+        <v>45479</v>
+      </c>
+      <c r="B1284" t="n">
+        <v>7221.52</v>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" s="3" t="n">
+        <v>45480</v>
+      </c>
+      <c r="B1285" t="n">
+        <v>7221.52</v>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" s="3" t="n">
+        <v>45481</v>
+      </c>
+      <c r="B1286" t="n">
+        <v>7221.52</v>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" s="3" t="n">
+        <v>45482</v>
+      </c>
+      <c r="B1287" t="n">
+        <v>7221.52</v>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" s="3" t="n">
+        <v>45483</v>
+      </c>
+      <c r="B1288" t="n">
+        <v>7224.079</v>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" s="3" t="n">
+        <v>45484</v>
+      </c>
+      <c r="B1289" t="n">
+        <v>7224.079</v>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" s="3" t="n">
+        <v>45485</v>
+      </c>
+      <c r="B1290" t="n">
+        <v>7224.079</v>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" s="3" t="n">
+        <v>45486</v>
+      </c>
+      <c r="B1291" t="n">
+        <v>7224.079</v>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" s="3" t="n">
+        <v>45487</v>
+      </c>
+      <c r="B1292" t="n">
+        <v>7224.079</v>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" s="3" t="n">
+        <v>45488</v>
+      </c>
+      <c r="B1293" t="n">
+        <v>7224.079</v>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" s="3" t="n">
+        <v>45489</v>
+      </c>
+      <c r="B1294" t="n">
+        <v>7224.079</v>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" s="3" t="n">
+        <v>45490</v>
+      </c>
+      <c r="B1295" t="n">
+        <v>7208.247</v>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" s="3" t="n">
+        <v>45491</v>
+      </c>
+      <c r="B1296" t="n">
+        <v>7208.247</v>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" s="3" t="n">
+        <v>45492</v>
+      </c>
+      <c r="B1297" t="n">
+        <v>7208.247</v>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" s="3" t="n">
+        <v>45493</v>
+      </c>
+      <c r="B1298" t="n">
+        <v>7208.247</v>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" s="3" t="n">
+        <v>45494</v>
+      </c>
+      <c r="B1299" t="n">
+        <v>7208.247</v>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" s="3" t="n">
+        <v>45495</v>
+      </c>
+      <c r="B1300" t="n">
+        <v>7208.247</v>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" s="3" t="n">
+        <v>45496</v>
+      </c>
+      <c r="B1301" t="n">
+        <v>7208.247</v>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" s="3" t="n">
+        <v>45497</v>
+      </c>
+      <c r="B1302" t="n">
+        <v>7205.455</v>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" s="3" t="n">
+        <v>45498</v>
+      </c>
+      <c r="B1303" t="n">
+        <v>7205.455</v>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" s="3" t="n">
+        <v>45499</v>
+      </c>
+      <c r="B1304" t="n">
+        <v>7205.455</v>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" s="3" t="n">
+        <v>45500</v>
+      </c>
+      <c r="B1305" t="n">
+        <v>7205.455</v>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" s="3" t="n">
+        <v>45501</v>
+      </c>
+      <c r="B1306" t="n">
+        <v>7205.455</v>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" s="3" t="n">
+        <v>45502</v>
+      </c>
+      <c r="B1307" t="n">
+        <v>7205.455</v>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" s="3" t="n">
+        <v>45503</v>
+      </c>
+      <c r="B1308" t="n">
+        <v>7205.455</v>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" s="3" t="n">
+        <v>45504</v>
+      </c>
+      <c r="B1309" t="n">
+        <v>7178.391</v>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" s="3" t="n">
+        <v>45505</v>
+      </c>
+      <c r="B1310" t="n">
+        <v>7178.391</v>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" s="3" t="n">
+        <v>45506</v>
+      </c>
+      <c r="B1311" t="n">
+        <v>7178.391</v>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" s="3" t="n">
+        <v>45507</v>
+      </c>
+      <c r="B1312" t="n">
+        <v>7178.391</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -32516,7 +33500,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1273"/>
+  <dimension ref="A1:B1312"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -42704,7 +43688,319 @@
         <v>45468</v>
       </c>
       <c r="B1273" t="n">
-        <v>435.916</v>
+        <v>466.31</v>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" s="3" t="n">
+        <v>45469</v>
+      </c>
+      <c r="B1274" t="n">
+        <v>490.156</v>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" s="3" t="n">
+        <v>45470</v>
+      </c>
+      <c r="B1275" t="n">
+        <v>531.692</v>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" s="3" t="n">
+        <v>45471</v>
+      </c>
+      <c r="B1276" t="n">
+        <v>664.5700000000001</v>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" s="3" t="n">
+        <v>45472</v>
+      </c>
+      <c r="B1277" t="n">
+        <v>664.5700000000001</v>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" s="3" t="n">
+        <v>45473</v>
+      </c>
+      <c r="B1278" t="n">
+        <v>664.5700000000001</v>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" s="3" t="n">
+        <v>45474</v>
+      </c>
+      <c r="B1279" t="n">
+        <v>451.783</v>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" s="3" t="n">
+        <v>45475</v>
+      </c>
+      <c r="B1280" t="n">
+        <v>443.369</v>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" s="3" t="n">
+        <v>45476</v>
+      </c>
+      <c r="B1281" t="n">
+        <v>425.898</v>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" s="3" t="n">
+        <v>45477</v>
+      </c>
+      <c r="B1282" t="n">
+        <v>425.898</v>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" s="3" t="n">
+        <v>45478</v>
+      </c>
+      <c r="B1283" t="n">
+        <v>390.632</v>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" s="3" t="n">
+        <v>45479</v>
+      </c>
+      <c r="B1284" t="n">
+        <v>390.632</v>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" s="3" t="n">
+        <v>45480</v>
+      </c>
+      <c r="B1285" t="n">
+        <v>390.632</v>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" s="3" t="n">
+        <v>45481</v>
+      </c>
+      <c r="B1286" t="n">
+        <v>415.257</v>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" s="3" t="n">
+        <v>45482</v>
+      </c>
+      <c r="B1287" t="n">
+        <v>423.152</v>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" s="3" t="n">
+        <v>45483</v>
+      </c>
+      <c r="B1288" t="n">
+        <v>422.147</v>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" s="3" t="n">
+        <v>45484</v>
+      </c>
+      <c r="B1289" t="n">
+        <v>403.708</v>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" s="3" t="n">
+        <v>45485</v>
+      </c>
+      <c r="B1290" t="n">
+        <v>406.59</v>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" s="3" t="n">
+        <v>45486</v>
+      </c>
+      <c r="B1291" t="n">
+        <v>406.59</v>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" s="3" t="n">
+        <v>45487</v>
+      </c>
+      <c r="B1292" t="n">
+        <v>406.59</v>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" s="3" t="n">
+        <v>45488</v>
+      </c>
+      <c r="B1293" t="n">
+        <v>413.28</v>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" s="3" t="n">
+        <v>45489</v>
+      </c>
+      <c r="B1294" t="n">
+        <v>409.594</v>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" s="3" t="n">
+        <v>45490</v>
+      </c>
+      <c r="B1295" t="n">
+        <v>399.401</v>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" s="3" t="n">
+        <v>45491</v>
+      </c>
+      <c r="B1296" t="n">
+        <v>391.652</v>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" s="3" t="n">
+        <v>45492</v>
+      </c>
+      <c r="B1297" t="n">
+        <v>379.801</v>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" s="3" t="n">
+        <v>45493</v>
+      </c>
+      <c r="B1298" t="n">
+        <v>379.801</v>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" s="3" t="n">
+        <v>45494</v>
+      </c>
+      <c r="B1299" t="n">
+        <v>379.801</v>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" s="3" t="n">
+        <v>45495</v>
+      </c>
+      <c r="B1300" t="n">
+        <v>395.901</v>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" s="3" t="n">
+        <v>45496</v>
+      </c>
+      <c r="B1301" t="n">
+        <v>389.837</v>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" s="3" t="n">
+        <v>45497</v>
+      </c>
+      <c r="B1302" t="n">
+        <v>399.121</v>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" s="3" t="n">
+        <v>45498</v>
+      </c>
+      <c r="B1303" t="n">
+        <v>377.433</v>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" s="3" t="n">
+        <v>45499</v>
+      </c>
+      <c r="B1304" t="n">
+        <v>381.257</v>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" s="3" t="n">
+        <v>45500</v>
+      </c>
+      <c r="B1305" t="n">
+        <v>381.257</v>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" s="3" t="n">
+        <v>45501</v>
+      </c>
+      <c r="B1306" t="n">
+        <v>381.257</v>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" s="3" t="n">
+        <v>45502</v>
+      </c>
+      <c r="B1307" t="n">
+        <v>385.281</v>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" s="3" t="n">
+        <v>45503</v>
+      </c>
+      <c r="B1308" t="n">
+        <v>367.054</v>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" s="3" t="n">
+        <v>45504</v>
+      </c>
+      <c r="B1309" t="n">
+        <v>413.2</v>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" s="3" t="n">
+        <v>45505</v>
+      </c>
+      <c r="B1310" t="n">
+        <v>348.885</v>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" s="3" t="n">
+        <v>45506</v>
+      </c>
+      <c r="B1311" t="n">
+        <v>338.473</v>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" s="3" t="n">
+        <v>45507</v>
+      </c>
+      <c r="B1312" t="n">
+        <v>338.473</v>
       </c>
     </row>
   </sheetData>
@@ -42718,7 +44014,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1273"/>
+  <dimension ref="A1:B1312"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -52898,7 +54194,7 @@
         <v>45467</v>
       </c>
       <c r="B1272" t="n">
-        <v>763.426</v>
+        <v>784.434</v>
       </c>
     </row>
     <row r="1273">
@@ -52906,7 +54202,319 @@
         <v>45468</v>
       </c>
       <c r="B1273" t="n">
-        <v>763.426</v>
+        <v>767.249</v>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" s="3" t="n">
+        <v>45469</v>
+      </c>
+      <c r="B1274" t="n">
+        <v>744.206</v>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" s="3" t="n">
+        <v>45470</v>
+      </c>
+      <c r="B1275" t="n">
+        <v>718.6180000000001</v>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" s="3" t="n">
+        <v>45471</v>
+      </c>
+      <c r="B1276" t="n">
+        <v>777.798</v>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" s="3" t="n">
+        <v>45472</v>
+      </c>
+      <c r="B1277" t="n">
+        <v>777.798</v>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" s="3" t="n">
+        <v>45473</v>
+      </c>
+      <c r="B1278" t="n">
+        <v>777.798</v>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" s="3" t="n">
+        <v>45474</v>
+      </c>
+      <c r="B1279" t="n">
+        <v>763.439</v>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" s="3" t="n">
+        <v>45475</v>
+      </c>
+      <c r="B1280" t="n">
+        <v>768.554</v>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" s="3" t="n">
+        <v>45476</v>
+      </c>
+      <c r="B1281" t="n">
+        <v>745.6079999999999</v>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" s="3" t="n">
+        <v>45477</v>
+      </c>
+      <c r="B1282" t="n">
+        <v>745.6079999999999</v>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" s="3" t="n">
+        <v>45478</v>
+      </c>
+      <c r="B1283" t="n">
+        <v>732.159</v>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" s="3" t="n">
+        <v>45479</v>
+      </c>
+      <c r="B1284" t="n">
+        <v>732.159</v>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" s="3" t="n">
+        <v>45480</v>
+      </c>
+      <c r="B1285" t="n">
+        <v>732.159</v>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" s="3" t="n">
+        <v>45481</v>
+      </c>
+      <c r="B1286" t="n">
+        <v>743.168</v>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" s="3" t="n">
+        <v>45482</v>
+      </c>
+      <c r="B1287" t="n">
+        <v>747.2380000000001</v>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" s="3" t="n">
+        <v>45483</v>
+      </c>
+      <c r="B1288" t="n">
+        <v>722.328</v>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" s="3" t="n">
+        <v>45484</v>
+      </c>
+      <c r="B1289" t="n">
+        <v>731.4160000000001</v>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" s="3" t="n">
+        <v>45485</v>
+      </c>
+      <c r="B1290" t="n">
+        <v>734.465</v>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" s="3" t="n">
+        <v>45486</v>
+      </c>
+      <c r="B1291" t="n">
+        <v>734.465</v>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" s="3" t="n">
+        <v>45487</v>
+      </c>
+      <c r="B1292" t="n">
+        <v>734.465</v>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" s="3" t="n">
+        <v>45488</v>
+      </c>
+      <c r="B1293" t="n">
+        <v>764.538</v>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" s="3" t="n">
+        <v>45489</v>
+      </c>
+      <c r="B1294" t="n">
+        <v>795.024</v>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" s="3" t="n">
+        <v>45490</v>
+      </c>
+      <c r="B1295" t="n">
+        <v>766.779</v>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" s="3" t="n">
+        <v>45491</v>
+      </c>
+      <c r="B1296" t="n">
+        <v>775.779</v>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" s="3" t="n">
+        <v>45492</v>
+      </c>
+      <c r="B1297" t="n">
+        <v>771.252</v>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" s="3" t="n">
+        <v>45493</v>
+      </c>
+      <c r="B1298" t="n">
+        <v>771.252</v>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" s="3" t="n">
+        <v>45494</v>
+      </c>
+      <c r="B1299" t="n">
+        <v>771.252</v>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" s="3" t="n">
+        <v>45495</v>
+      </c>
+      <c r="B1300" t="n">
+        <v>769.783</v>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" s="3" t="n">
+        <v>45496</v>
+      </c>
+      <c r="B1301" t="n">
+        <v>793.467</v>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" s="3" t="n">
+        <v>45497</v>
+      </c>
+      <c r="B1302" t="n">
+        <v>767.419</v>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" s="3" t="n">
+        <v>45498</v>
+      </c>
+      <c r="B1303" t="n">
+        <v>767.894</v>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" s="3" t="n">
+        <v>45499</v>
+      </c>
+      <c r="B1304" t="n">
+        <v>766.528</v>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" s="3" t="n">
+        <v>45500</v>
+      </c>
+      <c r="B1305" t="n">
+        <v>766.528</v>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" s="3" t="n">
+        <v>45501</v>
+      </c>
+      <c r="B1306" t="n">
+        <v>766.528</v>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" s="3" t="n">
+        <v>45502</v>
+      </c>
+      <c r="B1307" t="n">
+        <v>781.5</v>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" s="3" t="n">
+        <v>45503</v>
+      </c>
+      <c r="B1308" t="n">
+        <v>802.422</v>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" s="3" t="n">
+        <v>45504</v>
+      </c>
+      <c r="B1309" t="n">
+        <v>854.001</v>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" s="3" t="n">
+        <v>45505</v>
+      </c>
+      <c r="B1310" t="n">
+        <v>785.0940000000001</v>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" s="3" t="n">
+        <v>45506</v>
+      </c>
+      <c r="B1311" t="n">
+        <v>785.0940000000001</v>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" s="3" t="n">
+        <v>45507</v>
+      </c>
+      <c r="B1312" t="n">
+        <v>785.0940000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>